<commit_message>
fially fixed assessmet addig
</commit_message>
<xml_diff>
--- a/src/middlewares/excelFile.xlsx
+++ b/src/middlewares/excelFile.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="153222"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keyz\Desktop\readingspreadsheet\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\keyz\Documents\cbt\cbt-new\computer-based-assessment\excel examples\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -24,18 +24,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
-    <t>matric</t>
+    <t>who discovered mongo park?</t>
   </si>
   <si>
-    <t>ca</t>
+    <t>a</t>
   </si>
   <si>
-    <t>exam</t>
+    <t>a: Julius beger;b: Akpan;c: James;d: Titus;</t>
   </si>
   <si>
-    <t>13ms1023</t>
+    <t>natural sciences:mathematical sciences;</t>
   </si>
 </sst>
 </file>
@@ -353,34 +353,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="b">
+        <v>1</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
+      <c r="E1">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
+        <v>3</v>
+      </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="b">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
         <v>3</v>
-      </c>
-      <c r="B2">
-        <v>30</v>
-      </c>
-      <c r="C2">
-        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add level to user biodata info
</commit_message>
<xml_diff>
--- a/src/middlewares/excelFile.xlsx
+++ b/src/middlewares/excelFile.xlsx
@@ -24,21 +24,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="4">
   <si>
-    <t>13ms1023</t>
+    <t>who discovered mongo park?</t>
   </si>
   <si>
-    <t>16me1033</t>
+    <t>a</t>
   </si>
   <si>
-    <t>Emmanuel Menyaga</t>
+    <t>a: Julius beger;b: Akpan;c: James;d: Titus;</t>
   </si>
   <si>
-    <t>mathematical sciences</t>
-  </si>
-  <si>
-    <t>Ojonugwa Justice Alikali</t>
+    <t>natural sciences:mathematical sciences;</t>
   </si>
 </sst>
 </file>
@@ -356,40 +353,52 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D2"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="G5" sqref="G5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A1" t="b">
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="C1" t="s">
+      <c r="E1">
+        <v>9</v>
+      </c>
+      <c r="F1" t="s">
         <v>3</v>
       </c>
-      <c r="D1">
-        <v>30</v>
-      </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A2" t="b">
+        <v>1</v>
+      </c>
+      <c r="B2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
       <c r="C2" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" t="s">
+        <v>2</v>
+      </c>
+      <c r="E2">
+        <v>10</v>
+      </c>
+      <c r="F2" t="s">
         <v>3</v>
-      </c>
-      <c r="D2">
-        <v>30</v>
       </c>
     </row>
   </sheetData>

</xml_diff>